<commit_message>
Remove unneeded graph legend text. Add rental stress source.
</commit_message>
<xml_diff>
--- a/dashboard_loader/housing_rentalstress_uploader/housing_rentalstress.xlsx
+++ b/dashboard_loader/housing_rentalstress_uploader/housing_rentalstress.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="40">
   <si>
     <t xml:space="preserve">Reduce rental stress</t>
   </si>
@@ -138,6 +138,9 @@
   </si>
   <si>
     <t xml:space="preserve">ABS (unpublished), Survey of Income and Housing, various years.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Steering Committee for the Review of Government Service Provision (SCRGSP) 2018, Report on Government Services 2018, table GA.2.</t>
   </si>
 </sst>
 </file>
@@ -304,7 +307,7 @@
   </sheetPr>
   <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
     </sheetView>
   </sheetViews>
@@ -925,10 +928,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1017,6 +1020,11 @@
         <v>38</v>
       </c>
     </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>